<commit_message>
Cleaned up the diagrams a bit
</commit_message>
<xml_diff>
--- a/Expenses.xlsx
+++ b/Expenses.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cojoi_000\Documents\GitHub\Capstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanCardin\Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -77,9 +77,6 @@
     <t>https://www.sparkfun.com/categories/267</t>
   </si>
   <si>
-    <t>Project Estimate</t>
-  </si>
-  <si>
     <t>Cost Estimate Per Part</t>
   </si>
   <si>
@@ -138,6 +135,9 @@
   </si>
   <si>
     <t>https://www.sparkfun.com/products/9650</t>
+  </si>
+  <si>
+    <t>Totals</t>
   </si>
 </sst>
 </file>
@@ -147,7 +147,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +163,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -172,7 +180,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -198,45 +206,127 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -518,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,10 +620,10 @@
     <col min="2" max="2" width="29.85546875" style="5" customWidth="1"/>
     <col min="3" max="3" width="42.7109375" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="28.5703125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" style="25" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" style="5" customWidth="1"/>
     <col min="10" max="10" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -541,8 +631,8 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>18</v>
+      <c r="B1" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -553,277 +643,367 @@
       <c r="E1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="5"/>
+      <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="6">
         <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="3"/>
-      <c r="E2" s="15">
+      <c r="E2" s="10">
         <v>4</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="16">
+        <f>B2*E2</f>
         <v>40</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="K2" s="5"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="30"/>
+      <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="4">
+      <c r="A3" s="8"/>
+      <c r="B3" s="6">
         <v>20</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="3"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="8">
-        <v>80</v>
-      </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="16">
+        <f t="shared" ref="F3:F22" si="0">B3*E3</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="24"/>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="6">
         <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="10">
+      <c r="E4" s="12">
         <v>4</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="16">
+        <f>B4*E4</f>
         <v>40</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="6">
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="10">
+      <c r="E5" s="12">
         <v>4</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="16">
+        <f>B5*E5</f>
         <v>28</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="6">
         <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="10">
+      <c r="E6" s="12">
         <v>4</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="16">
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="30"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="6">
         <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="10">
+      <c r="E7" s="12">
         <v>4</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="16">
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="30"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="4">
+        <v>28</v>
+      </c>
+      <c r="B8" s="6">
         <v>13</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="10">
+      <c r="E8" s="12">
         <v>1</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="16">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="H8" s="3"/>
+      <c r="H8" s="30"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="10">
+      <c r="E9" s="12">
         <v>4</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="F9" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="24"/>
+      <c r="H9" s="30"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="6">
         <v>0.35</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="10">
+      <c r="E10" s="12">
         <v>4</v>
       </c>
-      <c r="F10" s="8">
-        <v>1.5</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="F10" s="16">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
+      <c r="G10" s="24"/>
+      <c r="H10" s="30"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="6">
         <v>42</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="10">
+      <c r="E11" s="12">
         <v>1</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="16">
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="30"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="6">
         <v>20</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="10">
+      <c r="E12" s="12">
         <v>1</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="16">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="30"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="4">
+        <v>29</v>
+      </c>
+      <c r="B13" s="6">
         <v>3</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="10">
+      <c r="E13" s="12">
         <v>1</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="16">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="17" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G13" s="24"/>
+      <c r="H13" s="30"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F14" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="31"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F15" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="31"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F16" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="31"/>
+    </row>
+    <row r="17" spans="1:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F17" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="31"/>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="4"/>
+      <c r="B18" s="6"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="10">
+      <c r="E18" s="12">
         <v>1</v>
       </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="3"/>
+      <c r="F18" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="24"/>
+      <c r="H18" s="31"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F19" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="31"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F20" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="31"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F21" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="31"/>
+    </row>
+    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F22" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="31"/>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="19"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="22">
+        <f>SUM(F2:F22)</f>
+        <v>247.4</v>
+      </c>
+      <c r="G23" s="26"/>
+      <c r="H23" s="27">
+        <f>SUM(H2:H22)</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Aug 13 meeting, updated Proposal and Cost sheet and added Presentation powerpoint
</commit_message>
<xml_diff>
--- a/Expenses.xlsx
+++ b/Expenses.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanCardin\Capstone\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25203"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12570"/>
+    <workbookView xWindow="740" yWindow="0" windowWidth="25200" windowHeight="12580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -24,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Part List</t>
   </si>
@@ -74,9 +72,6 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>https://www.sparkfun.com/categories/267</t>
-  </si>
-  <si>
     <t>Cost Estimate Per Part</t>
   </si>
   <si>
@@ -138,6 +133,12 @@
   </si>
   <si>
     <t>Totals</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/9716</t>
+  </si>
+  <si>
+    <t>Programming Board</t>
   </si>
 </sst>
 </file>
@@ -268,7 +269,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1"/>
@@ -283,14 +284,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -327,6 +322,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -388,7 +386,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -423,7 +421,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -600,7 +598,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -608,31 +606,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="42.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="13" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" style="17" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" style="25" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="42.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="11" customWidth="1"/>
+    <col min="6" max="6" width="28.5" style="15" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" style="23" customWidth="1"/>
+    <col min="8" max="8" width="21.83203125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="20" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>17</v>
+      <c r="B1" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -640,21 +638,21 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="23" t="s">
+      <c r="F1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="27" t="s">
         <v>7</v>
       </c>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15" thickTop="1">
       <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
@@ -662,355 +660,353 @@
         <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" s="3"/>
-      <c r="E2" s="10">
+      <c r="E2" s="9">
         <v>4</v>
       </c>
-      <c r="F2" s="16">
+      <c r="F2" s="14">
         <f>B2*E2</f>
         <v>40</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="30"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="28"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
       <c r="B3" s="6">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D3" s="3"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="16">
-        <f t="shared" ref="F3:F22" si="0">B3*E3</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="30"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E3" s="10">
+        <v>4</v>
+      </c>
+      <c r="F3" s="14">
+        <f>B3*E3</f>
+        <v>40</v>
+      </c>
+      <c r="G3" s="22"/>
+      <c r="H3" s="28"/>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="6">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="12">
+      <c r="E4" s="10">
         <v>4</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="14">
         <f>B4*E4</f>
-        <v>40</v>
-      </c>
-      <c r="G4" s="24"/>
-      <c r="H4" s="30"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="G4" s="22"/>
+      <c r="H4" s="28"/>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B5" s="6">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="10">
+        <v>4</v>
+      </c>
+      <c r="F5" s="14">
+        <f t="shared" ref="F5:F21" si="0">B5*E5</f>
+        <v>32</v>
+      </c>
+      <c r="G5" s="22"/>
+      <c r="H5" s="28"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="6">
         <v>7</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="10">
+        <v>4</v>
+      </c>
+      <c r="F6" s="14">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="G6" s="22"/>
+      <c r="H6" s="28"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="6">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="10">
+        <v>1</v>
+      </c>
+      <c r="F7" s="14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="H7" s="28"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="10">
+        <v>4</v>
+      </c>
+      <c r="F8" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="22"/>
+      <c r="H8" s="28"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0.35</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="10">
+        <v>4</v>
+      </c>
+      <c r="F9" s="14">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
+      <c r="G9" s="22"/>
+      <c r="H9" s="28"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="6">
+        <v>42</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="14">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="G10" s="22"/>
+      <c r="H10" s="28"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="6">
         <v>20</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="12">
-        <v>4</v>
-      </c>
-      <c r="F5" s="16">
-        <f>B5*E5</f>
+      <c r="C11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="10">
+        <v>1</v>
+      </c>
+      <c r="F11" s="14">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="G11" s="22"/>
+      <c r="H11" s="28"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="24"/>
-      <c r="H5" s="30"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="6">
-        <v>8</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B12" s="6">
+        <v>3</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="10">
+        <v>1</v>
+      </c>
+      <c r="F12" s="14">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G12" s="22"/>
+      <c r="H12" s="28"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="6">
+        <v>15</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="30">
+        <v>1</v>
+      </c>
+      <c r="F13" s="14">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="H13" s="29"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="F14" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="29"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="F15" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="29"/>
+    </row>
+    <row r="16" spans="1:11" ht="20" thickBot="1">
+      <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="12">
-        <v>4</v>
-      </c>
-      <c r="F6" s="16">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="G6" s="24"/>
-      <c r="H6" s="30"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="6">
-        <v>7</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="12">
-        <v>4</v>
-      </c>
-      <c r="F7" s="16">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="G7" s="24"/>
-      <c r="H7" s="30"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="6">
-        <v>13</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="12">
+      <c r="F16" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="29"/>
+    </row>
+    <row r="17" spans="1:11" ht="15" thickTop="1">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="10">
         <v>1</v>
       </c>
-      <c r="F8" s="16">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="H8" s="30"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="12">
-        <v>4</v>
-      </c>
-      <c r="F9" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="24"/>
-      <c r="H9" s="30"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="6">
-        <v>0.35</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="F17" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="22"/>
+      <c r="H17" s="29"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="F18" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="29"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="F19" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="29"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="F20" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="29"/>
+    </row>
+    <row r="21" spans="1:11" ht="15" thickBot="1">
+      <c r="F21" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="29"/>
+    </row>
+    <row r="22" spans="1:11" ht="15" thickBot="1">
+      <c r="A22" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="12">
-        <v>4</v>
-      </c>
-      <c r="F10" s="16">
-        <f t="shared" si="0"/>
-        <v>1.4</v>
-      </c>
-      <c r="G10" s="24"/>
-      <c r="H10" s="30"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="6">
-        <v>42</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="12">
-        <v>1</v>
-      </c>
-      <c r="F11" s="16">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="G11" s="24"/>
-      <c r="H11" s="30"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="6">
-        <v>20</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="12">
-        <v>1</v>
-      </c>
-      <c r="F12" s="16">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="G12" s="24"/>
-      <c r="H12" s="30"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="6">
-        <v>3</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="12">
-        <v>1</v>
-      </c>
-      <c r="F13" s="16">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G13" s="24"/>
-      <c r="H13" s="30"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F14" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="31"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F15" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="31"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F16" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="31"/>
-    </row>
-    <row r="17" spans="1:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H17" s="31"/>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="12">
-        <v>1</v>
-      </c>
-      <c r="F18" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="24"/>
-      <c r="H18" s="31"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F19" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H19" s="31"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F20" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H20" s="31"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F21" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H21" s="31"/>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H22" s="31"/>
-    </row>
-    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="22">
-        <f>SUM(F2:F22)</f>
-        <v>247.4</v>
-      </c>
-      <c r="G23" s="26"/>
-      <c r="H23" s="27">
-        <f>SUM(H2:H22)</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="20">
+        <f>SUM(F2:F21)</f>
+        <v>262.39999999999998</v>
+      </c>
+      <c r="G22" s="24"/>
+      <c r="H22" s="25">
+        <f>SUM(H2:H21)</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="E2:E3"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated expenses and Presentation
</commit_message>
<xml_diff>
--- a/Expenses.xlsx
+++ b/Expenses.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25203"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="0" windowWidth="25200" windowHeight="12580"/>
+    <workbookView xWindow="460" yWindow="0" windowWidth="25200" windowHeight="12580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>Part List</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Source</t>
   </si>
   <si>
-    <t>Part Name</t>
-  </si>
-  <si>
     <t>Arduino</t>
   </si>
   <si>
@@ -54,12 +51,6 @@
     <t>Transformer</t>
   </si>
   <si>
-    <t>Current Sensor</t>
-  </si>
-  <si>
-    <t>Switch/Button</t>
-  </si>
-  <si>
     <t>LED</t>
   </si>
   <si>
@@ -90,9 +81,6 @@
     <t>https://www.sparkfun.com/products/11042</t>
   </si>
   <si>
-    <t>Optional Parts</t>
-  </si>
-  <si>
     <t>http://www.amazon.com/Genuine-Authentic-Apple-Adapter-Charger/dp/B00QSB3UXE/ref=sr_1_cc_1?s=aps&amp;ie=UTF8&amp;qid=1437849720&amp;sr=1-1-catcorr&amp;keywords=apple+wall+charger</t>
   </si>
   <si>
@@ -102,9 +90,6 @@
     <t>http://www.amazon.com/Raspberry-Pi-Model-Project-Board/dp/B00T2U7R7I</t>
   </si>
   <si>
-    <t>Model B</t>
-  </si>
-  <si>
     <t>Micro SD Card</t>
   </si>
   <si>
@@ -114,21 +99,12 @@
     <t>http://www.amazon.com/SanDisk-Memory-Adapter-SDSDQUAN-032G-G4A-Version/dp/B00M55C0NS/ref=pd_bxgy_147_text_y</t>
   </si>
   <si>
-    <t>SanDisk Ultra 32GB</t>
-  </si>
-  <si>
     <t>http://www.amazon.com/Raspberry-Pi-Power-Supply-5v/dp/B00LSEOTYK</t>
   </si>
   <si>
-    <t>B+</t>
-  </si>
-  <si>
     <t>http://www.amazon.com/gp/product/B00JDVRCI0/ref=as_li_qf_sp_asin_il_tl?tag=htpcbeg-20&amp;ie=UTF8&amp;camp=1789&amp;creative=9325&amp;creativeASIN=B00JDVRCI0&amp;linkCode=as2&amp;linkId=2PT3YPZ25MGWJJ3P</t>
   </si>
   <si>
-    <t>Wireless N</t>
-  </si>
-  <si>
     <t>https://www.sparkfun.com/products/9650</t>
   </si>
   <si>
@@ -139,6 +115,18 @@
   </si>
   <si>
     <t>Programming Board</t>
+  </si>
+  <si>
+    <t>3D Printing Materials</t>
+  </si>
+  <si>
+    <t>http://library.northeastern.edu/services/3d-printing-studio</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/9190</t>
   </si>
 </sst>
 </file>
@@ -148,7 +136,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,6 +156,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -265,14 +269,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -325,9 +334,18 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="8">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -598,7 +616,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -606,399 +624,354 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection sqref="A1:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.1640625" customWidth="1"/>
-    <col min="2" max="2" width="29.83203125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="42.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.5" customWidth="1"/>
-    <col min="5" max="5" width="17.5" style="11" customWidth="1"/>
-    <col min="6" max="6" width="28.5" style="15" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" style="23" customWidth="1"/>
-    <col min="8" max="8" width="21.83203125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="10" customWidth="1"/>
+    <col min="4" max="4" width="28.5" style="14" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="42.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20" thickBot="1">
+    <row r="1" spans="1:9" ht="20" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickTop="1">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5">
+        <v>10</v>
+      </c>
+      <c r="C2" s="8">
+        <v>4</v>
+      </c>
+      <c r="D2" s="13">
+        <f>B2*C2</f>
+        <v>40</v>
+      </c>
+      <c r="E2" s="21"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5">
+        <v>10</v>
+      </c>
+      <c r="C3" s="9">
+        <v>4</v>
+      </c>
+      <c r="D3" s="13">
+        <f>B3*C3</f>
+        <v>40</v>
+      </c>
+      <c r="E3" s="21"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5">
+        <v>7</v>
+      </c>
+      <c r="C4" s="9">
+        <v>4</v>
+      </c>
+      <c r="D4" s="13">
+        <f>B4*C4</f>
+        <v>28</v>
+      </c>
+      <c r="E4" s="21"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5">
+        <v>8</v>
+      </c>
+      <c r="C5" s="9">
+        <v>4</v>
+      </c>
+      <c r="D5" s="13">
+        <f>B5*C5</f>
+        <v>32</v>
+      </c>
+      <c r="E5" s="21"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="5">
+        <v>7</v>
+      </c>
+      <c r="C6" s="9">
+        <v>4</v>
+      </c>
+      <c r="D6" s="13">
+        <f>B6*C6</f>
+        <v>28</v>
+      </c>
+      <c r="E6" s="21"/>
+      <c r="F6" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="5">
+        <v>13</v>
+      </c>
+      <c r="C7" s="9">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D7" s="13">
+        <f>B7*C7</f>
+        <v>13</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="9">
+        <v>4</v>
+      </c>
+      <c r="D8" s="13">
+        <f>B8*C8</f>
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E8" s="21"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0.35</v>
+      </c>
+      <c r="C9" s="9">
+        <v>4</v>
+      </c>
+      <c r="D9" s="13">
+        <f>B9*C9</f>
+        <v>1.4</v>
+      </c>
+      <c r="E9" s="21"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5">
+        <v>42</v>
+      </c>
+      <c r="C10" s="9">
+        <v>1</v>
+      </c>
+      <c r="D10" s="13">
+        <f>B10*C10</f>
+        <v>42</v>
+      </c>
+      <c r="E10" s="21"/>
+      <c r="F10" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5">
+        <v>20</v>
+      </c>
+      <c r="C11" s="9">
+        <v>1</v>
+      </c>
+      <c r="D11" s="13">
+        <f>B11*C11</f>
+        <v>20</v>
+      </c>
+      <c r="E11" s="21"/>
+      <c r="F11" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="5">
+        <v>3</v>
+      </c>
+      <c r="C12" s="9">
+        <v>1</v>
+      </c>
+      <c r="D12" s="13">
+        <f>B12*C12</f>
+        <v>3</v>
+      </c>
+      <c r="E12" s="21"/>
+      <c r="F12" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="5">
         <v>15</v>
       </c>
-      <c r="F1" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="4"/>
-    </row>
-    <row r="2" spans="1:11" ht="15" thickTop="1">
-      <c r="A2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="6">
-        <v>10</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="9">
-        <v>4</v>
-      </c>
-      <c r="F2" s="14">
-        <f>B2*E2</f>
-        <v>40</v>
-      </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="28"/>
-      <c r="K2" s="4"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="6">
-        <v>10</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="10">
-        <v>4</v>
-      </c>
-      <c r="F3" s="14">
-        <f>B3*E3</f>
-        <v>40</v>
-      </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="28"/>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="6">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="10">
-        <v>4</v>
-      </c>
-      <c r="F4" s="14">
-        <f>B4*E4</f>
+      <c r="C13" s="29">
+        <v>1</v>
+      </c>
+      <c r="D13" s="13">
+        <f>B13*C13</f>
+        <v>15</v>
+      </c>
+      <c r="F13" s="28"/>
+      <c r="G13" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15" thickBot="1">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="30">
+        <v>20</v>
+      </c>
+      <c r="C14" s="9">
+        <v>1</v>
+      </c>
+      <c r="D14" s="13">
+        <f>B14*C14</f>
+        <v>20</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" thickBot="1">
+      <c r="A15" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="22"/>
-      <c r="H4" s="28"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="6">
-        <v>8</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="10">
-        <v>4</v>
-      </c>
-      <c r="F5" s="14">
-        <f t="shared" ref="F5:F21" si="0">B5*E5</f>
-        <v>32</v>
-      </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="28"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="6">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="10">
-        <v>4</v>
-      </c>
-      <c r="F6" s="14">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="G6" s="22"/>
-      <c r="H6" s="28"/>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="6">
-        <v>13</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="10">
-        <v>1</v>
-      </c>
-      <c r="F7" s="14">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="H7" s="28"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="6">
+      <c r="B15" s="16"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="19">
+        <f>SUM(D2:D14)</f>
+        <v>284.39999999999998</v>
+      </c>
+      <c r="E15" s="23"/>
+      <c r="F15" s="24">
+        <f>SUM(F2:F14)</f>
         <v>0</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="10">
-        <v>4</v>
-      </c>
-      <c r="F8" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G8" s="22"/>
-      <c r="H8" s="28"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="6">
-        <v>0.35</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="10">
-        <v>4</v>
-      </c>
-      <c r="F9" s="14">
-        <f t="shared" si="0"/>
-        <v>1.4</v>
-      </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="28"/>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="6">
-        <v>42</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="10">
-        <v>1</v>
-      </c>
-      <c r="F10" s="14">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="28"/>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="6">
-        <v>20</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="10">
-        <v>1</v>
-      </c>
-      <c r="F11" s="14">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="G11" s="22"/>
-      <c r="H11" s="28"/>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="6">
-        <v>3</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="10">
-        <v>1</v>
-      </c>
-      <c r="F12" s="14">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G12" s="22"/>
-      <c r="H12" s="28"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="6">
-        <v>15</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="30">
-        <v>1</v>
-      </c>
-      <c r="F13" s="14">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="H13" s="29"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="F14" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="29"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="F15" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="29"/>
-    </row>
-    <row r="16" spans="1:11" ht="20" thickBot="1">
-      <c r="A16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="29"/>
-    </row>
-    <row r="17" spans="1:11" ht="15" thickTop="1">
-      <c r="A17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="10">
-        <v>1</v>
-      </c>
-      <c r="F17" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="22"/>
-      <c r="H17" s="29"/>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="F18" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="29"/>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="F19" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H19" s="29"/>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="F20" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H20" s="29"/>
-    </row>
-    <row r="21" spans="1:11" ht="15" thickBot="1">
-      <c r="F21" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H21" s="29"/>
-    </row>
-    <row r="22" spans="1:11" ht="15" thickBot="1">
-      <c r="A22" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="20">
-        <f>SUM(F2:F21)</f>
-        <v>262.39999999999998</v>
-      </c>
-      <c r="G22" s="24"/>
-      <c r="H22" s="25">
-        <f>SUM(H2:H21)</f>
-        <v>0</v>
-      </c>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>